<commit_message>
added ospar to table and tried to fix html
</commit_message>
<xml_diff>
--- a/data/Priority_IUCN.xlsx
+++ b/data/Priority_IUCN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pstephan\Documents\github\ConservationStatus\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53A0D8A-9D77-4517-BF74-86944070E74C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE3544F-1EDC-4D29-A1FD-03BD79525898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="203">
   <si>
     <t>Façade</t>
   </si>
@@ -49,6 +49,12 @@
     <t>Atlantique</t>
   </si>
   <si>
+    <t>Alopias superciliosus</t>
+  </si>
+  <si>
+    <t>Renard à gros yeux</t>
+  </si>
+  <si>
     <t>Alopias vulpinus</t>
   </si>
   <si>
@@ -88,15 +94,33 @@
     <t>Raie de Richardson</t>
   </si>
   <si>
+    <t>Carcharhinus plumbeus</t>
+  </si>
+  <si>
+    <t>Requin gris</t>
+  </si>
+  <si>
+    <t>Carcharodon carcharias</t>
+  </si>
+  <si>
+    <t>Grand requin blanc</t>
+  </si>
+  <si>
+    <t>Centrophorus granulosus</t>
+  </si>
+  <si>
+    <t>Requin-chagrin</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
     <t>Centrophorus squamosus</t>
   </si>
   <si>
     <t>Squale-chagrin de l'Atlantique</t>
   </si>
   <si>
-    <t>EN</t>
-  </si>
-  <si>
     <t>Centrophorus uyato</t>
   </si>
   <si>
@@ -220,6 +244,18 @@
     <t>Chien espagnol</t>
   </si>
   <si>
+    <t>Glaucostegus cemiculus</t>
+  </si>
+  <si>
+    <t>Raie-guitare fouisseuse</t>
+  </si>
+  <si>
+    <t>Gymnura altavela</t>
+  </si>
+  <si>
+    <t>Raie-papillon épineuse</t>
+  </si>
+  <si>
     <t>Harriotta raleighana</t>
   </si>
   <si>
@@ -280,6 +316,12 @@
     <t>Raie fleurie</t>
   </si>
   <si>
+    <t>Mitsukurina owstoni</t>
+  </si>
+  <si>
+    <t>Requin-lutin</t>
+  </si>
+  <si>
     <t>Mobula mobular</t>
   </si>
   <si>
@@ -292,12 +334,36 @@
     <t>Émissole tachetée</t>
   </si>
   <si>
+    <t>Mustelus mustelus</t>
+  </si>
+  <si>
+    <t>Émissole lisse</t>
+  </si>
+  <si>
+    <t>Mustelus punctulatus</t>
+  </si>
+  <si>
+    <t>Émissole pointillée</t>
+  </si>
+  <si>
     <t>Myliobatis aquila</t>
   </si>
   <si>
     <t>Aigle de mer</t>
   </si>
   <si>
+    <t>Odontaspis ferox</t>
+  </si>
+  <si>
+    <t>Requin-féroce</t>
+  </si>
+  <si>
+    <t>Oxynotus centrina</t>
+  </si>
+  <si>
+    <t>Centrine commune</t>
+  </si>
+  <si>
     <t>Oxynotus paradoxus</t>
   </si>
   <si>
@@ -310,6 +376,18 @@
     <t>Requin peau bleau</t>
   </si>
   <si>
+    <t>Pristis pectinata</t>
+  </si>
+  <si>
+    <t>Poisson-scie tident</t>
+  </si>
+  <si>
+    <t>Pristis pristis</t>
+  </si>
+  <si>
+    <t>Poisson-scie commun</t>
+  </si>
+  <si>
     <t>Pseudotriakis microdon</t>
   </si>
   <si>
@@ -340,6 +418,12 @@
     <t>Raie mêlée</t>
   </si>
   <si>
+    <t>Raja miraletus</t>
+  </si>
+  <si>
+    <t>Raie-miroir</t>
+  </si>
+  <si>
     <t>Raja montagui</t>
   </si>
   <si>
@@ -358,12 +442,24 @@
     <t>Raie ronde</t>
   </si>
   <si>
+    <t>Rhinobatos rhinobatos</t>
+  </si>
+  <si>
+    <t>Raie-guitare commune</t>
+  </si>
+  <si>
     <t>Rhinochimaera atlantica</t>
   </si>
   <si>
     <t>Chimère à nez mou</t>
   </si>
   <si>
+    <t>Rhinoptera marginata</t>
+  </si>
+  <si>
+    <t>Mourine lusitanienne</t>
+  </si>
+  <si>
     <t>Rostroraja alba</t>
   </si>
   <si>
@@ -400,12 +496,54 @@
     <t>Laimargue de Méditerranée</t>
   </si>
   <si>
+    <t>Sphyrna lewini</t>
+  </si>
+  <si>
+    <t>Requin-marteau halicorne</t>
+  </si>
+  <si>
+    <t>Sphyrna mokarran</t>
+  </si>
+  <si>
+    <t>Grand requin-marteau</t>
+  </si>
+  <si>
+    <t>Sphyrna zygaena</t>
+  </si>
+  <si>
+    <t>Requin-marteau commun</t>
+  </si>
+  <si>
+    <t>Squaliolus laticaudus</t>
+  </si>
+  <si>
+    <t>Squale nain</t>
+  </si>
+  <si>
     <t>Squalus acanthias</t>
   </si>
   <si>
     <t>Aiguillat commun</t>
   </si>
   <si>
+    <t>Squalus blainville</t>
+  </si>
+  <si>
+    <t>Aiguillat-coq</t>
+  </si>
+  <si>
+    <t>Squatina aculeata</t>
+  </si>
+  <si>
+    <t>Ange de mer épineux</t>
+  </si>
+  <si>
+    <t>Squatina oculata</t>
+  </si>
+  <si>
+    <t>Ange de mer ocellé</t>
+  </si>
+  <si>
     <t>Squatina squatina</t>
   </si>
   <si>
@@ -424,6 +562,18 @@
     <t>Torpille marbrée</t>
   </si>
   <si>
+    <t>Torpedo torpedo</t>
+  </si>
+  <si>
+    <t>Torpille ocellée</t>
+  </si>
+  <si>
+    <t>Zameus squamulosus</t>
+  </si>
+  <si>
+    <t>Squale-grogneur velouté</t>
+  </si>
+  <si>
     <t>Méditerranée</t>
   </si>
   <si>
@@ -433,12 +583,6 @@
     <t>Mourine vachette</t>
   </si>
   <si>
-    <t>Alopias superciliosus</t>
-  </si>
-  <si>
-    <t>Renard à gros yeux</t>
-  </si>
-  <si>
     <t>Bathytoshia centroura</t>
   </si>
   <si>
@@ -463,90 +607,18 @@
     <t>Requin bordé</t>
   </si>
   <si>
-    <t>Carcharhinus plumbeus</t>
-  </si>
-  <si>
-    <t>Requin gris</t>
-  </si>
-  <si>
     <t>Carcharias taurus</t>
   </si>
   <si>
     <t>Requin-taureau</t>
   </si>
   <si>
-    <t>Carcharodon carcharias</t>
-  </si>
-  <si>
-    <t>Grand requin blanc</t>
-  </si>
-  <si>
-    <t>Centrophorus granulosus</t>
-  </si>
-  <si>
-    <t>Requin-chagrin</t>
-  </si>
-  <si>
-    <t>Glaucostegus cemiculus</t>
-  </si>
-  <si>
-    <t>Raie-guitare fouisseuse</t>
-  </si>
-  <si>
-    <t>Gymnura altavela</t>
-  </si>
-  <si>
-    <t>Raie-papillon épineuse</t>
-  </si>
-  <si>
-    <t>Mustelus mustelus</t>
-  </si>
-  <si>
-    <t>Émissole lisse</t>
-  </si>
-  <si>
-    <t>Mustelus punctulatus</t>
-  </si>
-  <si>
-    <t>Émissole pointillée</t>
-  </si>
-  <si>
-    <t>Odontaspis ferox</t>
-  </si>
-  <si>
-    <t>Requin-féroce</t>
-  </si>
-  <si>
-    <t>Oxynotus centrina</t>
-  </si>
-  <si>
-    <t>Centrine commune</t>
-  </si>
-  <si>
-    <t>Pristis pectinata</t>
-  </si>
-  <si>
-    <t>Poisson-scie tident</t>
-  </si>
-  <si>
-    <t>Pristis pristis</t>
-  </si>
-  <si>
-    <t>Poisson-scie commun</t>
-  </si>
-  <si>
     <t>Raja asterias</t>
   </si>
   <si>
     <t>Raie etoilée</t>
   </si>
   <si>
-    <t>Raja miraletus</t>
-  </si>
-  <si>
-    <t>Raie-miroir</t>
-  </si>
-  <si>
     <t>Raja polystigma</t>
   </si>
   <si>
@@ -557,48 +629,6 @@
   </si>
   <si>
     <t>Raie râpe</t>
-  </si>
-  <si>
-    <t>Rhinobatos rhinobatos</t>
-  </si>
-  <si>
-    <t>Raie-guitare commune</t>
-  </si>
-  <si>
-    <t>Rhinoptera marginata</t>
-  </si>
-  <si>
-    <t>Mourine lusitanienne</t>
-  </si>
-  <si>
-    <t>Sphyrna zygaena</t>
-  </si>
-  <si>
-    <t>Requin-marteau commun</t>
-  </si>
-  <si>
-    <t>Squalus blainville</t>
-  </si>
-  <si>
-    <t>Aiguillat-coq</t>
-  </si>
-  <si>
-    <t>Squatina aculeata</t>
-  </si>
-  <si>
-    <t>Ange de mer épineux</t>
-  </si>
-  <si>
-    <t>Squatina oculata</t>
-  </si>
-  <si>
-    <t>Ange de mer ocellé</t>
-  </si>
-  <si>
-    <t>Torpedo torpedo</t>
-  </si>
-  <si>
-    <t>Torpille ocellée</t>
   </si>
 </sst>
 </file>
@@ -985,17 +1015,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H127"/>
+  <dimension ref="A1:H152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K105" sqref="K105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.21875" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1029,13 +1059,13 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -1047,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1055,13 +1085,13 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>167</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <v>6</v>
@@ -1081,13 +1111,13 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -1099,7 +1129,7 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1107,16 +1137,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1125,7 +1155,7 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1133,13 +1163,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -1159,13 +1189,13 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -1177,7 +1207,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1185,22 +1215,22 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1211,13 +1241,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -1226,7 +1256,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1237,25 +1267,25 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1263,19 +1293,19 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1289,19 +1319,19 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1315,25 +1345,25 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E13">
         <v>2</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1341,22 +1371,22 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1367,19 +1397,19 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1393,13 +1423,13 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="C16" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -1411,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1419,25 +1449,25 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>154</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>155</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1445,22 +1475,25 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>174</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>175</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1468,19 +1501,16 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1494,13 +1524,10 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1509,10 +1536,10 @@
         <v>2</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1520,13 +1547,13 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1546,19 +1573,19 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1572,10 +1599,13 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1595,13 +1625,13 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1613,7 +1643,7 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1621,13 +1651,13 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1636,10 +1666,10 @@
         <v>2</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1647,19 +1677,22 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>57</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -1670,19 +1703,16 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1696,25 +1726,25 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -1722,19 +1752,19 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="E29">
         <v>1</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -1748,13 +1778,10 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C30" t="s">
-        <v>87</v>
-      </c>
-      <c r="D30" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1774,19 +1801,19 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
       <c r="F31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -1800,19 +1827,19 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="C32" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="D32" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
       <c r="F32">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -1826,22 +1853,25 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>93</v>
+      </c>
+      <c r="D33" t="s">
+        <v>13</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33">
         <v>0</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -1849,25 +1879,25 @@
         <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34">
         <v>0</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -1875,25 +1905,25 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -1901,19 +1931,19 @@
         <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>105</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -1927,16 +1957,16 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>26</v>
+        <v>107</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1953,19 +1983,19 @@
         <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>109</v>
       </c>
       <c r="D38" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -1979,19 +2009,19 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -2005,19 +2035,19 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="C40" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="D40" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -2031,16 +2061,13 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
-        <v>57</v>
-      </c>
-      <c r="D41" t="s">
-        <v>11</v>
+        <v>119</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -2057,19 +2084,16 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>120</v>
       </c>
       <c r="C42" t="s">
-        <v>59</v>
-      </c>
-      <c r="D42" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -2083,16 +2107,16 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="C43" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="D43" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43">
         <v>2</v>
@@ -2101,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -2109,19 +2133,19 @@
         <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>66</v>
+        <v>136</v>
       </c>
       <c r="C44" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -2135,19 +2159,16 @@
         <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="C45" t="s">
-        <v>69</v>
-      </c>
-      <c r="D45" t="s">
-        <v>11</v>
+        <v>141</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -2161,25 +2182,25 @@
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>148</v>
       </c>
       <c r="C46" t="s">
-        <v>73</v>
+        <v>149</v>
       </c>
       <c r="D46" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G46">
         <v>0</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -2187,19 +2208,19 @@
         <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>170</v>
       </c>
       <c r="C47" t="s">
-        <v>75</v>
+        <v>171</v>
       </c>
       <c r="D47" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -2213,19 +2234,19 @@
         <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>172</v>
       </c>
       <c r="C48" t="s">
-        <v>89</v>
+        <v>173</v>
       </c>
       <c r="D48" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -2239,19 +2260,16 @@
         <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
-      </c>
-      <c r="D49" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -2265,13 +2283,13 @@
         <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="C50" t="s">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="D50" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -2291,13 +2309,13 @@
         <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="C51" t="s">
-        <v>95</v>
+        <v>21</v>
       </c>
       <c r="D51" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -2309,7 +2327,7 @@
         <v>0</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -2317,25 +2335,25 @@
         <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="C52" t="s">
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="D52" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E52">
         <v>0</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
       <c r="H52">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -2343,19 +2361,19 @@
         <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="C53" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="D53" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -2369,13 +2387,13 @@
         <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>104</v>
+        <v>35</v>
       </c>
       <c r="C54" t="s">
-        <v>105</v>
+        <v>36</v>
       </c>
       <c r="D54" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -2387,7 +2405,7 @@
         <v>0</v>
       </c>
       <c r="H54">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
@@ -2395,10 +2413,13 @@
         <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>110</v>
+        <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>111</v>
+        <v>48</v>
+      </c>
+      <c r="D55" t="s">
+        <v>13</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -2410,7 +2431,7 @@
         <v>0</v>
       </c>
       <c r="H55">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -2418,19 +2439,19 @@
         <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
       <c r="C56" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="D56" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E56">
         <v>0</v>
       </c>
       <c r="F56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -2444,13 +2465,13 @@
         <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="C57" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="D57" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -2462,7 +2483,7 @@
         <v>0</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
@@ -2470,13 +2491,13 @@
         <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="C58" t="s">
-        <v>121</v>
+        <v>73</v>
       </c>
       <c r="D58" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -2488,7 +2509,7 @@
         <v>0</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
@@ -2496,25 +2517,25 @@
         <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>124</v>
+        <v>78</v>
       </c>
       <c r="C59" t="s">
-        <v>125</v>
+        <v>79</v>
       </c>
       <c r="D59" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E59">
         <v>0</v>
       </c>
       <c r="F59">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G59">
         <v>0</v>
       </c>
       <c r="H59">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
@@ -2522,19 +2543,19 @@
         <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="C60" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="D60" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E60">
         <v>0</v>
       </c>
       <c r="F60">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -2548,19 +2569,19 @@
         <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>132</v>
+        <v>84</v>
       </c>
       <c r="C61" t="s">
-        <v>133</v>
+        <v>85</v>
       </c>
       <c r="D61" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="E61">
         <v>0</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -2571,25 +2592,25 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B62" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="C62" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="D62" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="E62">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -2597,19 +2618,16 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B63" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="C63" t="s">
-        <v>63</v>
-      </c>
-      <c r="D63" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="E63">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -2618,27 +2636,27 @@
         <v>0</v>
       </c>
       <c r="H63">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B64" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C64" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="D64" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E64">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -2649,22 +2667,22 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>189</v>
+        <v>102</v>
       </c>
       <c r="C65" t="s">
-        <v>190</v>
+        <v>103</v>
       </c>
       <c r="D65" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E65">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -2675,71 +2693,71 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B66" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C66" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="D66" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="E66">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G66">
         <v>0</v>
       </c>
       <c r="H66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B67" t="s">
-        <v>9</v>
+        <v>116</v>
       </c>
       <c r="C67" t="s">
-        <v>10</v>
+        <v>117</v>
       </c>
       <c r="D67" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="E67">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B68" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="C68" t="s">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="D68" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E68">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -2748,79 +2766,76 @@
         <v>0</v>
       </c>
       <c r="H68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B69" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="C69" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="D69" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E69">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B70" t="s">
-        <v>45</v>
+        <v>130</v>
       </c>
       <c r="C70" t="s">
-        <v>46</v>
+        <v>131</v>
       </c>
       <c r="D70" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="E70">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H70">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B71" t="s">
-        <v>50</v>
+        <v>132</v>
       </c>
       <c r="C71" t="s">
-        <v>51</v>
-      </c>
-      <c r="D71" t="s">
-        <v>11</v>
+        <v>133</v>
       </c>
       <c r="E71">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -2831,19 +2846,19 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="C72" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="E72">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -2854,22 +2869,22 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B73" t="s">
-        <v>88</v>
+        <v>142</v>
       </c>
       <c r="C73" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
       <c r="D73" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E73">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -2880,74 +2895,71 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B74" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="C74" t="s">
-        <v>160</v>
-      </c>
-      <c r="D74" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
       <c r="E74">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G74">
         <v>0</v>
       </c>
       <c r="H74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B75" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C75" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="D75" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F75">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G75">
         <v>0</v>
       </c>
       <c r="H75">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B76" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="C76" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="D76" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E76">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -2958,25 +2970,25 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B77" t="s">
-        <v>94</v>
+        <v>156</v>
       </c>
       <c r="C77" t="s">
-        <v>95</v>
+        <v>157</v>
       </c>
       <c r="D77" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="E77">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -2984,16 +2996,19 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B78" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="C78" t="s">
-        <v>180</v>
+        <v>159</v>
+      </c>
+      <c r="D78" t="s">
+        <v>13</v>
       </c>
       <c r="E78">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F78">
         <v>0</v>
@@ -3002,24 +3017,24 @@
         <v>0</v>
       </c>
       <c r="H78">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B79" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="C79" t="s">
-        <v>115</v>
+        <v>161</v>
       </c>
       <c r="D79" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="E79">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -3033,68 +3048,71 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B80" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C80" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
       <c r="D80" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E80">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G80">
         <v>0</v>
       </c>
       <c r="H80">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B81" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
       <c r="C81" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="D81" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E81">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G81">
         <v>0</v>
       </c>
       <c r="H81">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B82" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="C82" t="s">
-        <v>136</v>
+        <v>169</v>
+      </c>
+      <c r="D82" t="s">
+        <v>13</v>
       </c>
       <c r="E82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F82">
         <v>0</v>
@@ -3108,19 +3126,22 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B83" t="s">
-        <v>137</v>
+        <v>176</v>
       </c>
       <c r="C83" t="s">
-        <v>138</v>
+        <v>177</v>
+      </c>
+      <c r="D83" t="s">
+        <v>13</v>
       </c>
       <c r="E83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F83">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -3131,22 +3152,22 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B84" t="s">
-        <v>141</v>
+        <v>178</v>
       </c>
       <c r="C84" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="D84" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -3157,51 +3178,51 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B85" t="s">
-        <v>147</v>
+        <v>180</v>
       </c>
       <c r="C85" t="s">
-        <v>148</v>
+        <v>181</v>
       </c>
       <c r="D85" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G85">
         <v>0</v>
       </c>
       <c r="H85">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B86" t="s">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="C86" t="s">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c r="D86" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F86">
         <v>0</v>
       </c>
       <c r="G86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H86">
         <v>0</v>
@@ -3209,19 +3230,19 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B87" t="s">
+        <v>42</v>
+      </c>
+      <c r="C87" t="s">
         <v>43</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
         <v>44</v>
       </c>
-      <c r="D87" t="s">
-        <v>11</v>
-      </c>
       <c r="E87">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F87">
         <v>0</v>
@@ -3235,45 +3256,45 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B88" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="C88" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D88" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="E88">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F88">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G88">
         <v>0</v>
       </c>
       <c r="H88">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B89" t="s">
-        <v>56</v>
+        <v>172</v>
       </c>
       <c r="C89" t="s">
-        <v>57</v>
+        <v>173</v>
       </c>
       <c r="D89" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E89">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F89">
         <v>0</v>
@@ -3287,19 +3308,19 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B90" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="C90" t="s">
-        <v>158</v>
+        <v>196</v>
       </c>
       <c r="D90" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E90">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F90">
         <v>0</v>
@@ -3308,27 +3329,27 @@
         <v>0</v>
       </c>
       <c r="H90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B91" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="C91" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="D91" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E91">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -3339,16 +3360,16 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B92" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C92" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E92">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F92">
         <v>0</v>
@@ -3357,56 +3378,56 @@
         <v>0</v>
       </c>
       <c r="H92">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B93" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="C93" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="D93" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E93">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G93">
         <v>0</v>
       </c>
       <c r="H93">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B94" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="C94" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="D94" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E94">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H94">
         <v>0</v>
@@ -3414,22 +3435,22 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B95" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="C95" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="D95" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E95">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -3440,25 +3461,25 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B96" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="C96" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="D96" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E96">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F96">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H96">
         <v>0</v>
@@ -3466,25 +3487,22 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B97" t="s">
-        <v>163</v>
+        <v>140</v>
       </c>
       <c r="C97" t="s">
-        <v>164</v>
-      </c>
-      <c r="D97" t="s">
-        <v>11</v>
+        <v>141</v>
       </c>
       <c r="E97">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F97">
         <v>0</v>
       </c>
       <c r="G97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H97">
         <v>0</v>
@@ -3492,19 +3510,19 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B98" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="C98" t="s">
-        <v>93</v>
+        <v>147</v>
       </c>
       <c r="D98" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="E98">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F98">
         <v>0</v>
@@ -3518,16 +3536,19 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B99" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C99" t="s">
-        <v>168</v>
+        <v>171</v>
+      </c>
+      <c r="D99" t="s">
+        <v>13</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F99">
         <v>0</v>
@@ -3536,21 +3557,24 @@
         <v>0</v>
       </c>
       <c r="H99">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B100" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C100" t="s">
-        <v>170</v>
+        <v>175</v>
+      </c>
+      <c r="D100" t="s">
+        <v>61</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F100">
         <v>0</v>
@@ -3564,51 +3588,51 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B101" t="s">
-        <v>102</v>
+        <v>11</v>
       </c>
       <c r="C101" t="s">
-        <v>103</v>
+        <v>12</v>
       </c>
       <c r="D101" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="E101">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F101">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H101">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B102" t="s">
-        <v>183</v>
+        <v>24</v>
       </c>
       <c r="C102" t="s">
-        <v>184</v>
+        <v>25</v>
       </c>
       <c r="D102" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E102">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F102">
         <v>0</v>
       </c>
       <c r="G102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H102">
         <v>0</v>
@@ -3616,25 +3640,25 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B103" t="s">
-        <v>139</v>
+        <v>53</v>
       </c>
       <c r="C103" t="s">
-        <v>140</v>
+        <v>54</v>
       </c>
       <c r="D103" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E103">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F103">
         <v>1</v>
       </c>
       <c r="G103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H103">
         <v>0</v>
@@ -3642,19 +3666,19 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B104" t="s">
-        <v>143</v>
+        <v>58</v>
       </c>
       <c r="C104" t="s">
-        <v>144</v>
+        <v>59</v>
       </c>
       <c r="D104" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E104">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F104">
         <v>0</v>
@@ -3668,19 +3692,19 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B105" t="s">
-        <v>145</v>
+        <v>76</v>
       </c>
       <c r="C105" t="s">
-        <v>146</v>
+        <v>77</v>
       </c>
       <c r="D105" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F105">
         <v>0</v>
@@ -3694,123 +3718,117 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B106" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="C106" t="s">
-        <v>31</v>
-      </c>
-      <c r="D106" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="E106">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F106">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G106">
         <v>0</v>
       </c>
       <c r="H106">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B107" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="C107" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="D107" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E107">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F107">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G107">
         <v>0</v>
       </c>
       <c r="H107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B108" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="C108" t="s">
-        <v>61</v>
+        <v>111</v>
       </c>
       <c r="D108" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E108">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F108">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G108">
         <v>0</v>
       </c>
       <c r="H108">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B109" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="C109" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="D109" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E109">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F109">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H109">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B110" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="C110" t="s">
-        <v>69</v>
-      </c>
-      <c r="D110" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="E110">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F110">
         <v>0</v>
@@ -3824,19 +3842,19 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B111" t="s">
-        <v>84</v>
+        <v>166</v>
       </c>
       <c r="C111" t="s">
-        <v>85</v>
+        <v>167</v>
       </c>
       <c r="D111" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E111">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F111">
         <v>1</v>
@@ -3850,22 +3868,19 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B112" t="s">
-        <v>98</v>
+        <v>185</v>
       </c>
       <c r="C112" t="s">
-        <v>99</v>
-      </c>
-      <c r="D112" t="s">
-        <v>47</v>
+        <v>186</v>
       </c>
       <c r="E112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -3876,22 +3891,19 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B113" t="s">
-        <v>171</v>
+        <v>9</v>
       </c>
       <c r="C113" t="s">
-        <v>172</v>
-      </c>
-      <c r="D113" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -3902,25 +3914,25 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B114" t="s">
-        <v>100</v>
+        <v>189</v>
       </c>
       <c r="C114" t="s">
-        <v>101</v>
+        <v>190</v>
       </c>
       <c r="D114" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H114">
         <v>0</v>
@@ -3928,65 +3940,71 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B115" t="s">
-        <v>173</v>
+        <v>28</v>
       </c>
       <c r="C115" t="s">
-        <v>174</v>
+        <v>29</v>
+      </c>
+      <c r="D115" t="s">
+        <v>30</v>
       </c>
       <c r="E115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F115">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H115">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B116" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="C116" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="D116" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F116">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G116">
         <v>0</v>
       </c>
       <c r="H116">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B117" t="s">
-        <v>175</v>
+        <v>62</v>
       </c>
       <c r="C117" t="s">
-        <v>176</v>
+        <v>63</v>
+      </c>
+      <c r="D117" t="s">
+        <v>37</v>
       </c>
       <c r="E117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F117">
         <v>2</v>
@@ -3995,24 +4013,24 @@
         <v>0</v>
       </c>
       <c r="H117">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B118" t="s">
-        <v>177</v>
+        <v>64</v>
       </c>
       <c r="C118" t="s">
-        <v>178</v>
+        <v>65</v>
       </c>
       <c r="D118" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F118">
         <v>0</v>
@@ -4026,22 +4044,22 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B119" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="C119" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="D119" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F119">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -4052,48 +4070,51 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B120" t="s">
-        <v>181</v>
+        <v>90</v>
       </c>
       <c r="C120" t="s">
-        <v>182</v>
+        <v>91</v>
+      </c>
+      <c r="D120" t="s">
+        <v>30</v>
       </c>
       <c r="E120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G120">
         <v>0</v>
       </c>
       <c r="H120">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B121" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="C121" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="D121" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="E121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F121">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H121">
         <v>0</v>
@@ -4101,48 +4122,48 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B122" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="C122" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="D122" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="E122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F122">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G122">
         <v>0</v>
       </c>
       <c r="H122">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B123" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C123" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D123" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F123">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -4153,22 +4174,22 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B124" t="s">
-        <v>185</v>
+        <v>114</v>
       </c>
       <c r="C124" t="s">
-        <v>186</v>
+        <v>115</v>
       </c>
       <c r="D124" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G124">
         <v>0</v>
@@ -4179,19 +4200,16 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B125" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C125" t="s">
-        <v>131</v>
-      </c>
-      <c r="D125" t="s">
-        <v>11</v>
+        <v>119</v>
       </c>
       <c r="E125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F125">
         <v>0</v>
@@ -4200,27 +4218,27 @@
         <v>0</v>
       </c>
       <c r="H125">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="B126" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C126" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D126" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E126">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F126">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G126">
         <v>0</v>
@@ -4231,35 +4249,676 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
+        <v>184</v>
+      </c>
+      <c r="B127" t="s">
+        <v>162</v>
+      </c>
+      <c r="C127" t="s">
+        <v>163</v>
+      </c>
+      <c r="D127" t="s">
+        <v>13</v>
+      </c>
+      <c r="E127">
+        <v>1</v>
+      </c>
+      <c r="F127">
+        <v>0</v>
+      </c>
+      <c r="G127">
+        <v>1</v>
+      </c>
+      <c r="H127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>184</v>
+      </c>
+      <c r="B128" t="s">
+        <v>187</v>
+      </c>
+      <c r="C128" t="s">
+        <v>188</v>
+      </c>
+      <c r="D128" t="s">
+        <v>13</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128">
+        <v>1</v>
+      </c>
+      <c r="G128">
+        <v>0</v>
+      </c>
+      <c r="H128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>184</v>
+      </c>
+      <c r="B129" t="s">
+        <v>191</v>
+      </c>
+      <c r="C129" t="s">
+        <v>192</v>
+      </c>
+      <c r="D129" t="s">
+        <v>13</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129">
+        <v>0</v>
+      </c>
+      <c r="G129">
+        <v>0</v>
+      </c>
+      <c r="H129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>184</v>
+      </c>
+      <c r="B130" t="s">
+        <v>193</v>
+      </c>
+      <c r="C130" t="s">
+        <v>194</v>
+      </c>
+      <c r="D130" t="s">
+        <v>13</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130">
+        <v>0</v>
+      </c>
+      <c r="G130">
+        <v>0</v>
+      </c>
+      <c r="H130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>184</v>
+      </c>
+      <c r="B131" t="s">
+        <v>38</v>
+      </c>
+      <c r="C131" t="s">
+        <v>39</v>
+      </c>
+      <c r="D131" t="s">
+        <v>13</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+      <c r="F131">
+        <v>3</v>
+      </c>
+      <c r="G131">
+        <v>0</v>
+      </c>
+      <c r="H131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>184</v>
+      </c>
+      <c r="B132" t="s">
+        <v>45</v>
+      </c>
+      <c r="C132" t="s">
+        <v>46</v>
+      </c>
+      <c r="D132" t="s">
+        <v>13</v>
+      </c>
+      <c r="E132">
+        <v>0</v>
+      </c>
+      <c r="F132">
+        <v>4</v>
+      </c>
+      <c r="G132">
+        <v>0</v>
+      </c>
+      <c r="H132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>184</v>
+      </c>
+      <c r="B133" t="s">
+        <v>68</v>
+      </c>
+      <c r="C133" t="s">
+        <v>69</v>
+      </c>
+      <c r="D133" t="s">
+        <v>13</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+      <c r="F133">
+        <v>3</v>
+      </c>
+      <c r="G133">
+        <v>0</v>
+      </c>
+      <c r="H133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>184</v>
+      </c>
+      <c r="B134" t="s">
+        <v>72</v>
+      </c>
+      <c r="C134" t="s">
+        <v>73</v>
+      </c>
+      <c r="D134" t="s">
+        <v>55</v>
+      </c>
+      <c r="E134">
+        <v>0</v>
+      </c>
+      <c r="F134">
+        <v>4</v>
+      </c>
+      <c r="G134">
+        <v>0</v>
+      </c>
+      <c r="H134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>184</v>
+      </c>
+      <c r="B135" t="s">
+        <v>80</v>
+      </c>
+      <c r="C135" t="s">
+        <v>81</v>
+      </c>
+      <c r="D135" t="s">
+        <v>13</v>
+      </c>
+      <c r="E135">
+        <v>0</v>
+      </c>
+      <c r="F135">
+        <v>0</v>
+      </c>
+      <c r="G135">
+        <v>0</v>
+      </c>
+      <c r="H135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>184</v>
+      </c>
+      <c r="B136" t="s">
+        <v>96</v>
+      </c>
+      <c r="C136" t="s">
+        <v>97</v>
+      </c>
+      <c r="D136" t="s">
+        <v>44</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+      <c r="F136">
+        <v>2</v>
+      </c>
+      <c r="G136">
+        <v>0</v>
+      </c>
+      <c r="H136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>184</v>
+      </c>
+      <c r="B137" t="s">
+        <v>124</v>
+      </c>
+      <c r="C137" t="s">
+        <v>125</v>
+      </c>
+      <c r="D137" t="s">
+        <v>55</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="F137">
+        <v>3</v>
+      </c>
+      <c r="G137">
+        <v>0</v>
+      </c>
+      <c r="H137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>184</v>
+      </c>
+      <c r="B138" t="s">
+        <v>197</v>
+      </c>
+      <c r="C138" t="s">
+        <v>198</v>
+      </c>
+      <c r="D138" t="s">
+        <v>13</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="F138">
+        <v>3</v>
+      </c>
+      <c r="G138">
+        <v>0</v>
+      </c>
+      <c r="H138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>184</v>
+      </c>
+      <c r="B139" t="s">
+        <v>126</v>
+      </c>
+      <c r="C139" t="s">
+        <v>127</v>
+      </c>
+      <c r="D139" t="s">
+        <v>13</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="F139">
+        <v>1</v>
+      </c>
+      <c r="G139">
+        <v>0</v>
+      </c>
+      <c r="H139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>184</v>
+      </c>
+      <c r="B140" t="s">
+        <v>132</v>
+      </c>
+      <c r="C140" t="s">
+        <v>133</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <v>4</v>
+      </c>
+      <c r="G140">
+        <v>0</v>
+      </c>
+      <c r="H140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>184</v>
+      </c>
+      <c r="B141" t="s">
         <v>134</v>
       </c>
-      <c r="B127" t="s">
-        <v>191</v>
-      </c>
-      <c r="C127" t="s">
-        <v>192</v>
-      </c>
-      <c r="D127" t="s">
-        <v>11</v>
-      </c>
-      <c r="E127">
-        <v>0</v>
-      </c>
-      <c r="F127">
-        <v>2</v>
-      </c>
-      <c r="G127">
-        <v>0</v>
-      </c>
-      <c r="H127">
+      <c r="C141" t="s">
+        <v>135</v>
+      </c>
+      <c r="D141" t="s">
+        <v>13</v>
+      </c>
+      <c r="E141">
+        <v>0</v>
+      </c>
+      <c r="F141">
+        <v>3</v>
+      </c>
+      <c r="G141">
+        <v>0</v>
+      </c>
+      <c r="H141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>184</v>
+      </c>
+      <c r="B142" t="s">
+        <v>199</v>
+      </c>
+      <c r="C142" t="s">
+        <v>200</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="F142">
+        <v>2</v>
+      </c>
+      <c r="G142">
+        <v>0</v>
+      </c>
+      <c r="H142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>184</v>
+      </c>
+      <c r="B143" t="s">
+        <v>201</v>
+      </c>
+      <c r="C143" t="s">
+        <v>202</v>
+      </c>
+      <c r="D143" t="s">
+        <v>13</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143">
+        <v>0</v>
+      </c>
+      <c r="G143">
+        <v>0</v>
+      </c>
+      <c r="H143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>184</v>
+      </c>
+      <c r="B144" t="s">
+        <v>136</v>
+      </c>
+      <c r="C144" t="s">
+        <v>137</v>
+      </c>
+      <c r="D144" t="s">
+        <v>13</v>
+      </c>
+      <c r="E144">
+        <v>0</v>
+      </c>
+      <c r="F144">
+        <v>1</v>
+      </c>
+      <c r="G144">
+        <v>0</v>
+      </c>
+      <c r="H144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>184</v>
+      </c>
+      <c r="B145" t="s">
+        <v>144</v>
+      </c>
+      <c r="C145" t="s">
+        <v>145</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145">
+        <v>0</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+      <c r="H145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>184</v>
+      </c>
+      <c r="B146" t="s">
+        <v>148</v>
+      </c>
+      <c r="C146" t="s">
+        <v>149</v>
+      </c>
+      <c r="D146" t="s">
+        <v>55</v>
+      </c>
+      <c r="E146">
+        <v>0</v>
+      </c>
+      <c r="F146">
+        <v>3</v>
+      </c>
+      <c r="G146">
+        <v>0</v>
+      </c>
+      <c r="H146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>184</v>
+      </c>
+      <c r="B147" t="s">
+        <v>150</v>
+      </c>
+      <c r="C147" t="s">
+        <v>151</v>
+      </c>
+      <c r="D147" t="s">
+        <v>55</v>
+      </c>
+      <c r="E147">
+        <v>0</v>
+      </c>
+      <c r="F147">
+        <v>2</v>
+      </c>
+      <c r="G147">
+        <v>0</v>
+      </c>
+      <c r="H147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>184</v>
+      </c>
+      <c r="B148" t="s">
+        <v>156</v>
+      </c>
+      <c r="C148" t="s">
+        <v>157</v>
+      </c>
+      <c r="D148" t="s">
+        <v>13</v>
+      </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
+      <c r="F148">
+        <v>1</v>
+      </c>
+      <c r="G148">
+        <v>0</v>
+      </c>
+      <c r="H148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>184</v>
+      </c>
+      <c r="B149" t="s">
+        <v>168</v>
+      </c>
+      <c r="C149" t="s">
+        <v>169</v>
+      </c>
+      <c r="D149" t="s">
+        <v>13</v>
+      </c>
+      <c r="E149">
+        <v>0</v>
+      </c>
+      <c r="F149">
+        <v>1</v>
+      </c>
+      <c r="G149">
+        <v>0</v>
+      </c>
+      <c r="H149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>184</v>
+      </c>
+      <c r="B150" t="s">
+        <v>176</v>
+      </c>
+      <c r="C150" t="s">
+        <v>177</v>
+      </c>
+      <c r="D150" t="s">
+        <v>13</v>
+      </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
+      <c r="F150">
+        <v>0</v>
+      </c>
+      <c r="G150">
+        <v>0</v>
+      </c>
+      <c r="H150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>184</v>
+      </c>
+      <c r="B151" t="s">
+        <v>178</v>
+      </c>
+      <c r="C151" t="s">
+        <v>179</v>
+      </c>
+      <c r="D151" t="s">
+        <v>55</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+      <c r="F151">
+        <v>3</v>
+      </c>
+      <c r="G151">
+        <v>0</v>
+      </c>
+      <c r="H151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>184</v>
+      </c>
+      <c r="B152" t="s">
+        <v>180</v>
+      </c>
+      <c r="C152" t="s">
+        <v>181</v>
+      </c>
+      <c r="D152" t="s">
+        <v>13</v>
+      </c>
+      <c r="E152">
+        <v>0</v>
+      </c>
+      <c r="F152">
+        <v>2</v>
+      </c>
+      <c r="G152">
+        <v>0</v>
+      </c>
+      <c r="H152">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H127">
-    <sortCondition ref="A2:A127"/>
-    <sortCondition descending="1" ref="E2:E127"/>
-    <sortCondition ref="B2:B127"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H152">
+    <sortCondition ref="A2:A152"/>
+    <sortCondition descending="1" ref="E2:E152"/>
+    <sortCondition ref="B2:B152"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>